<commit_message>
Python prefer underscore over dots in names
</commit_message>
<xml_diff>
--- a/data/df_splited.xlsx
+++ b/data/df_splited.xlsx
@@ -7,12 +7,12 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="train.data" sheetId="1" r:id="rId1"/>
-    <sheet name="test.data" sheetId="2" r:id="rId2"/>
-    <sheet name="train.data.prep" sheetId="3" r:id="rId3"/>
-    <sheet name="test.data.prep" sheetId="4" r:id="rId4"/>
-    <sheet name="train.data.bc" sheetId="5" r:id="rId5"/>
-    <sheet name="test.data.bc" sheetId="6" r:id="rId6"/>
+    <sheet name="train_data" sheetId="1" r:id="rId1"/>
+    <sheet name="test_data" sheetId="2" r:id="rId2"/>
+    <sheet name="train_data_prep" sheetId="3" r:id="rId3"/>
+    <sheet name="test_data_prep" sheetId="4" r:id="rId4"/>
+    <sheet name="train_data_bc" sheetId="5" r:id="rId5"/>
+    <sheet name="test_data_bc" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>